<commit_message>
finished until ex 29
</commit_message>
<xml_diff>
--- a/task_24b2.xlsx
+++ b/task_24b2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="60" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="30" uniqueCount="11">
   <si>
     <t>Number</t>
   </si>
@@ -23,25 +23,25 @@
     <t>First name</t>
   </si>
   <si>
-    <t>Dorka</t>
-  </si>
-  <si>
-    <t>Alejandro</t>
-  </si>
-  <si>
-    <t>Ryan</t>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Wernher</t>
+  </si>
+  <si>
+    <t>Szergej</t>
   </si>
   <si>
     <t>Surname</t>
   </si>
   <si>
-    <t>Zomok</t>
-  </si>
-  <si>
-    <t>Novoa</t>
-  </si>
-  <si>
-    <t>Boggio</t>
+    <t>Sagan</t>
+  </si>
+  <si>
+    <t>von Braun</t>
+  </si>
+  <si>
+    <t>Koroljov</t>
   </si>
   <si>
     <t>Age</t>
@@ -101,8 +101,8 @@
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="true"/>
     <col min="2" max="2" width="10.28515625" customWidth="true"/>
-    <col min="3" max="3" width="9" customWidth="true"/>
-    <col min="4" max="4" width="5.140625" customWidth="true"/>
+    <col min="3" max="3" width="10" customWidth="true"/>
+    <col min="4" max="4" width="4.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="0">
-        <v>1000</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4">
@@ -158,7 +158,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="0">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -175,8 +175,8 @@
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="true"/>
     <col min="2" max="2" width="10.42578125" customWidth="true"/>
-    <col min="3" max="3" width="9" customWidth="true"/>
-    <col min="4" max="4" width="5.140625" customWidth="true"/>
+    <col min="3" max="3" width="10" customWidth="true"/>
+    <col min="4" max="4" width="4.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -218,7 +218,7 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>1000</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4">
@@ -232,7 +232,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>98</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -249,63 +249,63 @@
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="true"/>
     <col min="2" max="2" width="10.28515625" customWidth="true"/>
-    <col min="3" max="3" width="9" customWidth="true"/>
-    <col min="4" max="4" width="5.140625" customWidth="true"/>
+    <col min="3" max="3" width="10" customWidth="true"/>
+    <col min="4" max="4" width="4.5703125" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="0" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="0">
-        <v>2</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0">
-        <v>1000</v>
+      <c r="D2">
+        <v>88</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="0">
-        <v>3</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0">
-        <v>98</v>
+      <c r="D3">
+        <v>71</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>67</v>
       </c>
     </row>

</xml_diff>